<commit_message>
aded taskModule method & created new class file
</commit_message>
<xml_diff>
--- a/SG_Maven_Project/TestData/taskModule.xlsx
+++ b/SG_Maven_Project/TestData/taskModule.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
+    <sheet name="Tasks" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
@@ -342,7 +342,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>

</xml_diff>